<commit_message>
implementacao do schedule, teste de confirmacao de email e comentarios
</commit_message>
<xml_diff>
--- a/emails.xlsx
+++ b/emails.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,11 @@
           <t>Nome</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>ConfirmationID</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -492,6 +497,7 @@
           <t>daniel</t>
         </is>
       </c>
+      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -518,6 +524,11 @@
       <c r="F3" t="inlineStr">
         <is>
           <t>daniel</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>94a8008e-c7ed-4642-9526-df6ed7af3261</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
remover pessoa apos 7 dias se o email nao foi confirmado
</commit_message>
<xml_diff>
--- a/emails.xlsx
+++ b/emails.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,6 +469,11 @@
           <t>ConfirmationID</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>DataEnvioInicial</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -498,6 +503,7 @@
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -507,30 +513,49 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>brinquedo batman</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>daniel.jmendes2@gmail.com</t>
-        </is>
-      </c>
+          <t>brinquedo superman</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
           <t>n</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Teste excelTeste excel</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>brinquedo superman</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>daniel.jmendes2@gmail.com</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
         <is>
           <t>daniel</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>bfe934ae-921b-4a84-870a-c75aeb9aab9e</t>
-        </is>
-      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>